<commit_message>
wrapped excel workbook save in try statement to handle permission error when workbook is open
</commit_message>
<xml_diff>
--- a/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
+++ b/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
@@ -420,6 +420,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="40" customWidth="1" min="1" max="1"/>
+    <col width="100" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">

</xml_diff>

<commit_message>
added font styling to room cell and line to open excel file after saving
</commit_message>
<xml_diff>
--- a/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
+++ b/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
@@ -17,13 +17,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="16"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +50,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,59 +432,59 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="40" customWidth="1" min="1" max="1"/>
-    <col width="100" customWidth="1" min="2" max="2"/>
+    <col width="60" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>RH1 Kitchen</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -484,105 +494,105 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>RH1 Bath</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>RH1 Master Bath</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Vanity Filler - R</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>RH2 Kitchen</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -592,60 +602,60 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -655,81 +665,81 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="1" t="inlineStr">
         <is>
           <t>RH2 Bath</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">RH2 Master Bath </t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="1" t="inlineStr">
         <is>
           <t>RH3 Kitchen</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -739,60 +749,60 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -802,81 +812,81 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="1" t="inlineStr">
         <is>
           <t>RH3 Bath</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="2" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="1" t="inlineStr">
         <is>
           <t>RH3 Master Bath</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="1" t="inlineStr">
         <is>
           <t>RH4 Kitchen</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="2" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -886,60 +896,60 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B54" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -949,81 +959,81 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" s="1" t="inlineStr">
         <is>
           <t>RH4 Bath</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58" s="2" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B58" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" s="1" t="inlineStr">
         <is>
           <t>RH4 Master Bath</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="A64" s="1" t="inlineStr">
         <is>
           <t>RH5 Kitchen</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
+      <c r="A65" s="2" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B65" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
+      <c r="A66" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B66" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1033,60 +1043,60 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="B67" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
+      <c r="A69" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B69" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="B70" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B71" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1096,81 +1106,81 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
+      <c r="A73" s="1" t="inlineStr">
         <is>
           <t>RH5 Bath</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
+      <c r="A74" s="2" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B74" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
+      <c r="A75" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B75" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
+      <c r="A77" s="1" t="inlineStr">
         <is>
           <t>RH5 Master Bath</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
+      <c r="A78" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B78" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
+      <c r="A80" s="1" t="inlineStr">
         <is>
           <t>RH6 Kitchen</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
+      <c r="A81" s="2" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B81" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
+      <c r="A82" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B82" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1180,60 +1190,60 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
+      <c r="A83" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B83" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
+      <c r="A85" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B85" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
+      <c r="A86" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="B86" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
+      <c r="A87" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B87" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1243,81 +1253,81 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
+      <c r="A89" s="1" t="inlineStr">
         <is>
           <t>RH6 Bath</t>
         </is>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
+      <c r="A90" s="2" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="B90" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
+      <c r="A91" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B91" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
+      <c r="A93" s="1" t="inlineStr">
         <is>
           <t>RH6 Master Bath</t>
         </is>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
+      <c r="A96" s="1" t="inlineStr">
         <is>
           <t>RH7 Kitchen</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
+      <c r="A97" s="2" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr">
+      <c r="B97" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
+      <c r="A98" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr">
+      <c r="B98" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1327,60 +1337,60 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
+      <c r="A99" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="B99" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
+      <c r="A101" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B101" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
+      <c r="A102" s="2" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr">
+      <c r="B102" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
+      <c r="A103" s="2" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr">
+      <c r="B103" s="2" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1390,50 +1400,50 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
+      <c r="A105" s="1" t="inlineStr">
         <is>
           <t>RH7 Bath</t>
         </is>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr">
+      <c r="A106" s="2" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
+      <c r="B106" s="2" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
+      <c r="A107" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B107" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
+      <c r="A109" s="1" t="inlineStr">
         <is>
           <t>RH7 Master Bath</t>
         </is>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
+      <c r="A110" s="2" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B110" s="2" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>

</xml_diff>

<commit_message>
layout of report is generally good, need to add room and cabinet numbers
</commit_message>
<xml_diff>
--- a/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
+++ b/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet'!$A$1:$C$133</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet'!$A$1:$B$133</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -30,6 +30,7 @@
     <font>
       <b val="1"/>
       <sz val="16"/>
+      <u val="single"/>
     </font>
     <font>
       <i val="1"/>
@@ -47,13 +48,23 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="00D4D4D4"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -64,11 +75,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,7 +455,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="58" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
added cabinet numbers to each line
</commit_message>
<xml_diff>
--- a/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
+++ b/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet'!$A$1:$B$134</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet'!$A$1:$C$134</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -75,7 +75,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -86,8 +86,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B132"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +469,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="58" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -486,55 +493,80 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>R1N1</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>R1N5</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>R1N2</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>R1N4</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -544,12 +576,17 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>R1N9</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -568,31 +605,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="A12" s="5" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>R2N1</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="inlineStr">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>R2N3</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -611,31 +663,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="inlineStr">
+      <c r="A17" s="5" t="inlineStr">
         <is>
           <t>Vanity Filler - R</t>
         </is>
       </c>
-      <c r="B17" s="4" t="inlineStr">
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>R3N2</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B18" s="4" t="inlineStr">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t>R3N3</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -654,31 +721,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr">
+      <c r="A22" s="5" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B22" s="4" t="inlineStr">
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>R4N1</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="inlineStr">
+      <c r="A23" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B23" s="4" t="inlineStr">
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>R4N4</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -688,60 +770,85 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="inlineStr">
+      <c r="A24" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B24" s="4" t="inlineStr">
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>R4N2</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B25" s="4" t="inlineStr">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>R4N5</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B26" s="4" t="inlineStr">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>R4N10</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="inlineStr">
+      <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B27" s="4" t="inlineStr">
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>R4N8</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="inlineStr">
+      <c r="A28" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B28" s="4" t="inlineStr">
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>R4N9</t>
+        </is>
+      </c>
+      <c r="C28" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -763,31 +870,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B31" s="3" t="inlineStr">
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="inlineStr">
+      <c r="A32" s="5" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B32" s="4" t="inlineStr">
+      <c r="B32" s="6" t="inlineStr">
+        <is>
+          <t>R5N1</t>
+        </is>
+      </c>
+      <c r="C32" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B33" s="4" t="inlineStr">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>R5N3</t>
+        </is>
+      </c>
+      <c r="C33" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -806,19 +928,29 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B36" s="3" t="inlineStr">
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B37" s="4" t="inlineStr">
+      <c r="A37" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t>R6N3</t>
+        </is>
+      </c>
+      <c r="C37" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -837,31 +969,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B40" s="3" t="inlineStr">
+      <c r="B40" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="inlineStr">
+      <c r="A41" s="5" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B41" s="4" t="inlineStr">
+      <c r="B41" s="6" t="inlineStr">
+        <is>
+          <t>R7N1</t>
+        </is>
+      </c>
+      <c r="C41" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="inlineStr">
+      <c r="A42" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B42" s="4" t="inlineStr">
+      <c r="B42" s="6" t="inlineStr">
+        <is>
+          <t>R7N4</t>
+        </is>
+      </c>
+      <c r="C42" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -871,60 +1018,85 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="inlineStr">
+      <c r="A43" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B43" s="4" t="inlineStr">
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>R7N2</t>
+        </is>
+      </c>
+      <c r="C43" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B44" s="4" t="inlineStr">
+      <c r="A44" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B44" s="6" t="inlineStr">
+        <is>
+          <t>R7N5</t>
+        </is>
+      </c>
+      <c r="C44" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B45" s="4" t="inlineStr">
+      <c r="A45" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>R7N10</t>
+        </is>
+      </c>
+      <c r="C45" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="inlineStr">
+      <c r="A46" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B46" s="4" t="inlineStr">
+      <c r="B46" s="6" t="inlineStr">
+        <is>
+          <t>R7N8</t>
+        </is>
+      </c>
+      <c r="C46" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="inlineStr">
+      <c r="A47" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B47" s="4" t="inlineStr">
+      <c r="B47" s="6" t="inlineStr">
+        <is>
+          <t>R7N9</t>
+        </is>
+      </c>
+      <c r="C47" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -946,31 +1118,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B50" s="3" t="inlineStr">
+      <c r="B50" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="inlineStr">
+      <c r="A51" s="5" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B51" s="4" t="inlineStr">
+      <c r="B51" s="6" t="inlineStr">
+        <is>
+          <t>R8N1</t>
+        </is>
+      </c>
+      <c r="C51" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B52" s="4" t="inlineStr">
+      <c r="A52" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B52" s="6" t="inlineStr">
+        <is>
+          <t>R8N3</t>
+        </is>
+      </c>
+      <c r="C52" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -989,19 +1176,29 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B55" s="3" t="inlineStr">
+      <c r="B55" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B56" s="4" t="inlineStr">
+      <c r="A56" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B56" s="6" t="inlineStr">
+        <is>
+          <t>R9C3</t>
+        </is>
+      </c>
+      <c r="C56" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -1020,31 +1217,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B59" s="3" t="inlineStr">
+      <c r="B59" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C59" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="4" t="inlineStr">
+      <c r="A60" s="5" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B60" s="4" t="inlineStr">
+      <c r="B60" s="6" t="inlineStr">
+        <is>
+          <t>R10N1</t>
+        </is>
+      </c>
+      <c r="C60" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="4" t="inlineStr">
+      <c r="A61" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B61" s="4" t="inlineStr">
+      <c r="B61" s="6" t="inlineStr">
+        <is>
+          <t>R10N4</t>
+        </is>
+      </c>
+      <c r="C61" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1054,60 +1266,85 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="4" t="inlineStr">
+      <c r="A62" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B62" s="4" t="inlineStr">
+      <c r="B62" s="6" t="inlineStr">
+        <is>
+          <t>R10N2</t>
+        </is>
+      </c>
+      <c r="C62" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B63" s="4" t="inlineStr">
+      <c r="A63" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B63" s="6" t="inlineStr">
+        <is>
+          <t>R10N5</t>
+        </is>
+      </c>
+      <c r="C63" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B64" s="4" t="inlineStr">
+      <c r="A64" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B64" s="6" t="inlineStr">
+        <is>
+          <t>R10N10</t>
+        </is>
+      </c>
+      <c r="C64" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="4" t="inlineStr">
+      <c r="A65" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B65" s="4" t="inlineStr">
+      <c r="B65" s="6" t="inlineStr">
+        <is>
+          <t>R10N8</t>
+        </is>
+      </c>
+      <c r="C65" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="4" t="inlineStr">
+      <c r="A66" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B66" s="4" t="inlineStr">
+      <c r="B66" s="6" t="inlineStr">
+        <is>
+          <t>R10N9</t>
+        </is>
+      </c>
+      <c r="C66" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1129,31 +1366,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B69" s="3" t="inlineStr">
+      <c r="B69" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="4" t="inlineStr">
+      <c r="A70" s="5" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B70" s="4" t="inlineStr">
+      <c r="B70" s="6" t="inlineStr">
+        <is>
+          <t>R11N1</t>
+        </is>
+      </c>
+      <c r="C70" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B71" s="4" t="inlineStr">
+      <c r="A71" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B71" s="6" t="inlineStr">
+        <is>
+          <t>R11N3</t>
+        </is>
+      </c>
+      <c r="C71" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -1172,19 +1424,29 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B74" s="3" t="inlineStr">
+      <c r="B74" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B75" s="4" t="inlineStr">
+      <c r="A75" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B75" s="6" t="inlineStr">
+        <is>
+          <t>R12N3</t>
+        </is>
+      </c>
+      <c r="C75" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -1203,31 +1465,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B78" s="3" t="inlineStr">
+      <c r="B78" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C78" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="4" t="inlineStr">
+      <c r="A79" s="5" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B79" s="4" t="inlineStr">
+      <c r="B79" s="6" t="inlineStr">
+        <is>
+          <t>R13N1</t>
+        </is>
+      </c>
+      <c r="C79" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="4" t="inlineStr">
+      <c r="A80" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B80" s="4" t="inlineStr">
+      <c r="B80" s="6" t="inlineStr">
+        <is>
+          <t>R13N4</t>
+        </is>
+      </c>
+      <c r="C80" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1237,60 +1514,85 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="4" t="inlineStr">
+      <c r="A81" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B81" s="4" t="inlineStr">
+      <c r="B81" s="6" t="inlineStr">
+        <is>
+          <t>R13N2</t>
+        </is>
+      </c>
+      <c r="C81" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B82" s="4" t="inlineStr">
+      <c r="A82" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B82" s="6" t="inlineStr">
+        <is>
+          <t>R13N5</t>
+        </is>
+      </c>
+      <c r="C82" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B83" s="4" t="inlineStr">
+      <c r="A83" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B83" s="6" t="inlineStr">
+        <is>
+          <t>R13N10</t>
+        </is>
+      </c>
+      <c r="C83" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="4" t="inlineStr">
+      <c r="A84" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B84" s="4" t="inlineStr">
+      <c r="B84" s="6" t="inlineStr">
+        <is>
+          <t>R13N8</t>
+        </is>
+      </c>
+      <c r="C84" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="4" t="inlineStr">
+      <c r="A85" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B85" s="4" t="inlineStr">
+      <c r="B85" s="6" t="inlineStr">
+        <is>
+          <t>R13N9</t>
+        </is>
+      </c>
+      <c r="C85" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1312,31 +1614,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B88" s="3" t="inlineStr">
+      <c r="B88" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C88" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="4" t="inlineStr">
+      <c r="A89" s="5" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B89" s="4" t="inlineStr">
+      <c r="B89" s="6" t="inlineStr">
+        <is>
+          <t>R14N1</t>
+        </is>
+      </c>
+      <c r="C89" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B90" s="4" t="inlineStr">
+      <c r="A90" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B90" s="6" t="inlineStr">
+        <is>
+          <t>R14N3</t>
+        </is>
+      </c>
+      <c r="C90" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -1355,19 +1672,29 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B93" s="3" t="inlineStr">
+      <c r="B93" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B94" s="4" t="inlineStr">
+      <c r="A94" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B94" s="6" t="inlineStr">
+        <is>
+          <t>R15N3</t>
+        </is>
+      </c>
+      <c r="C94" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -1386,31 +1713,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B97" s="3" t="inlineStr">
+      <c r="B97" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="4" t="inlineStr">
+      <c r="A98" s="5" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B98" s="4" t="inlineStr">
+      <c r="B98" s="6" t="inlineStr">
+        <is>
+          <t>R16N1</t>
+        </is>
+      </c>
+      <c r="C98" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="4" t="inlineStr">
+      <c r="A99" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B99" s="4" t="inlineStr">
+      <c r="B99" s="6" t="inlineStr">
+        <is>
+          <t>R16N4</t>
+        </is>
+      </c>
+      <c r="C99" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1420,60 +1762,85 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="4" t="inlineStr">
+      <c r="A100" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B100" s="4" t="inlineStr">
+      <c r="B100" s="6" t="inlineStr">
+        <is>
+          <t>R16N2</t>
+        </is>
+      </c>
+      <c r="C100" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B101" s="4" t="inlineStr">
+      <c r="A101" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B101" s="6" t="inlineStr">
+        <is>
+          <t>R16N5</t>
+        </is>
+      </c>
+      <c r="C101" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B102" s="4" t="inlineStr">
+      <c r="A102" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B102" s="6" t="inlineStr">
+        <is>
+          <t>R16N10</t>
+        </is>
+      </c>
+      <c r="C102" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="4" t="inlineStr">
+      <c r="A103" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B103" s="4" t="inlineStr">
+      <c r="B103" s="6" t="inlineStr">
+        <is>
+          <t>R16N8</t>
+        </is>
+      </c>
+      <c r="C103" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="4" t="inlineStr">
+      <c r="A104" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B104" s="4" t="inlineStr">
+      <c r="B104" s="6" t="inlineStr">
+        <is>
+          <t>R16N9</t>
+        </is>
+      </c>
+      <c r="C104" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1495,31 +1862,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B107" s="3" t="inlineStr">
+      <c r="B107" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="4" t="inlineStr">
+      <c r="A108" s="5" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B108" s="4" t="inlineStr">
+      <c r="B108" s="6" t="inlineStr">
+        <is>
+          <t>R17N1</t>
+        </is>
+      </c>
+      <c r="C108" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B109" s="4" t="inlineStr">
+      <c r="A109" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B109" s="6" t="inlineStr">
+        <is>
+          <t>R17N3</t>
+        </is>
+      </c>
+      <c r="C109" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -1538,19 +1920,29 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B112" s="3" t="inlineStr">
+      <c r="B112" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C112" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B113" s="4" t="inlineStr">
+      <c r="A113" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B113" s="6" t="inlineStr">
+        <is>
+          <t>R18N3</t>
+        </is>
+      </c>
+      <c r="C113" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -1569,31 +1961,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B116" s="3" t="inlineStr">
+      <c r="B116" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C116" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="4" t="inlineStr">
+      <c r="A117" s="5" t="inlineStr">
         <is>
           <t>Base Filler - L</t>
         </is>
       </c>
-      <c r="B117" s="4" t="inlineStr">
+      <c r="B117" s="6" t="inlineStr">
+        <is>
+          <t>R19N1</t>
+        </is>
+      </c>
+      <c r="C117" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="4" t="inlineStr">
+      <c r="A118" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B118" s="4" t="inlineStr">
+      <c r="B118" s="6" t="inlineStr">
+        <is>
+          <t>R19N4</t>
+        </is>
+      </c>
+      <c r="C118" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1603,60 +2010,85 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="4" t="inlineStr">
+      <c r="A119" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B119" s="4" t="inlineStr">
+      <c r="B119" s="6" t="inlineStr">
+        <is>
+          <t>R19N2</t>
+        </is>
+      </c>
+      <c r="C119" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B120" s="4" t="inlineStr">
+      <c r="A120" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B120" s="6" t="inlineStr">
+        <is>
+          <t>R19N5</t>
+        </is>
+      </c>
+      <c r="C120" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B121" s="4" t="inlineStr">
+      <c r="A121" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B121" s="6" t="inlineStr">
+        <is>
+          <t>R19N10</t>
+        </is>
+      </c>
+      <c r="C121" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="4" t="inlineStr">
+      <c r="A122" s="5" t="inlineStr">
         <is>
           <t>Wall Filler - L</t>
         </is>
       </c>
-      <c r="B122" s="4" t="inlineStr">
+      <c r="B122" s="6" t="inlineStr">
+        <is>
+          <t>R19N8</t>
+        </is>
+      </c>
+      <c r="C122" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="4" t="inlineStr">
+      <c r="A123" s="5" t="inlineStr">
         <is>
           <t>Light Valance (107)</t>
         </is>
       </c>
-      <c r="B123" s="4" t="inlineStr">
+      <c r="B123" s="6" t="inlineStr">
+        <is>
+          <t>R19N9</t>
+        </is>
+      </c>
+      <c r="C123" s="5" t="inlineStr">
         <is>
           <t>"L" shaped product with face height equal to Height dimension.
 Use cutoff for cleat. Pocketscrew cleat on B side.
@@ -1678,31 +2110,46 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B126" s="3" t="inlineStr">
+      <c r="B126" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C126" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="4" t="inlineStr">
+      <c r="A127" s="5" t="inlineStr">
         <is>
           <t>Vanity Filler - L</t>
         </is>
       </c>
-      <c r="B127" s="4" t="inlineStr">
+      <c r="B127" s="6" t="inlineStr">
+        <is>
+          <t>R20N1</t>
+        </is>
+      </c>
+      <c r="C127" s="5" t="inlineStr">
         <is>
           <t>Pocketscrew B-side of cleat every ~8"</t>
         </is>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B128" s="4" t="inlineStr">
+      <c r="A128" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B128" s="6" t="inlineStr">
+        <is>
+          <t>R20N3</t>
+        </is>
+      </c>
+      <c r="C128" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -1721,19 +2168,29 @@
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B131" s="3" t="inlineStr">
+      <c r="B131" s="4" t="inlineStr">
+        <is>
+          <t>CabNo</t>
+        </is>
+      </c>
+      <c r="C131" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="4" t="inlineStr">
-        <is>
-          <t>Toeboard</t>
-        </is>
-      </c>
-      <c r="B132" s="4" t="inlineStr">
+      <c r="A132" s="5" t="inlineStr">
+        <is>
+          <t>Toeboard</t>
+        </is>
+      </c>
+      <c r="B132" s="6" t="inlineStr">
+        <is>
+          <t>R21N3</t>
+        </is>
+      </c>
+      <c r="C132" s="5" t="inlineStr">
         <is>
           <t>leave long, even if product width says otherwise</t>
         </is>
@@ -1741,28 +2198,28 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="A96:C96"/>
+    <mergeCell ref="A106:C106"/>
+    <mergeCell ref="A111:C111"/>
+    <mergeCell ref="A115:C115"/>
+    <mergeCell ref="A125:C125"/>
+    <mergeCell ref="A130:C130"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
changed font sizes and added room number to room name
</commit_message>
<xml_diff>
--- a/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
+++ b/ISO 394-02 - Test Job/ISO 394-02 - Test Job.xlsx
@@ -42,7 +42,7 @@
       <sz val="12"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,13 +84,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" indent="2"/>
+      <alignment horizontal="general" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1" indent="2"/>
+      <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>RH1 Kitchen</t>
+          <t>RH1 Kitchen (Room1)</t>
         </is>
       </c>
     </row>
@@ -595,7 +595,7 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>RH1 Bath</t>
+          <t>RH1 Bath (Room2)</t>
         </is>
       </c>
     </row>
@@ -653,7 +653,7 @@
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>RH1 Master Bath</t>
+          <t>RH1 Master Bath (Room3)</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>RH2 Kitchen</t>
+          <t>RH2 Kitchen (Room4)</t>
         </is>
       </c>
     </row>
@@ -860,7 +860,7 @@
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>RH2 Bath</t>
+          <t>RH2 Bath (Room5)</t>
         </is>
       </c>
     </row>
@@ -918,7 +918,7 @@
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">RH2 Master Bath </t>
+          <t>RH2 Master Bath  (Room6)</t>
         </is>
       </c>
     </row>
@@ -959,7 +959,7 @@
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>RH3 Kitchen</t>
+          <t>RH3 Kitchen (Room7)</t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>RH3 Bath</t>
+          <t>RH3 Bath (Room8)</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>RH3 Master Bath</t>
+          <t>RH3 Master Bath (Room9)</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>RH4 Kitchen</t>
+          <t>RH4 Kitchen (Room10)</t>
         </is>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>RH4 Bath</t>
+          <t>RH4 Bath (Room11)</t>
         </is>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
     <row r="73">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>RH4 Master Bath</t>
+          <t>RH4 Master Bath (Room12)</t>
         </is>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
     <row r="77">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>RH5 Kitchen</t>
+          <t>RH5 Kitchen (Room13)</t>
         </is>
       </c>
     </row>
@@ -1604,7 +1604,7 @@
     <row r="87">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>RH5 Bath</t>
+          <t>RH5 Bath (Room14)</t>
         </is>
       </c>
     </row>
@@ -1662,7 +1662,7 @@
     <row r="92">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>RH5 Master Bath</t>
+          <t>RH5 Master Bath (Room15)</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
     <row r="96">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>RH6 Kitchen</t>
+          <t>RH6 Kitchen (Room16)</t>
         </is>
       </c>
     </row>
@@ -1852,7 +1852,7 @@
     <row r="106">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>RH6 Bath</t>
+          <t>RH6 Bath (Room17)</t>
         </is>
       </c>
     </row>
@@ -1910,7 +1910,7 @@
     <row r="111">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>RH6 Master Bath</t>
+          <t>RH6 Master Bath (Room18)</t>
         </is>
       </c>
     </row>
@@ -1951,7 +1951,7 @@
     <row r="115">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>RH7 Kitchen</t>
+          <t>RH7 Kitchen (Room19)</t>
         </is>
       </c>
     </row>
@@ -2100,7 +2100,7 @@
     <row r="125">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>RH7 Bath</t>
+          <t>RH7 Bath (Room20)</t>
         </is>
       </c>
     </row>
@@ -2158,7 +2158,7 @@
     <row r="130">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>RH7 Master Bath</t>
+          <t>RH7 Master Bath (Room21)</t>
         </is>
       </c>
     </row>

</xml_diff>